<commit_message>
working just set screen TO larger that shoot interval
</commit_message>
<xml_diff>
--- a/bandwith_calculation_cctv_image_android.xlsx
+++ b/bandwith_calculation_cctv_image_android.xlsx
@@ -404,7 +404,7 @@
   <dimension ref="D4:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,14 +482,14 @@
     </row>
     <row r="6" spans="4:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="3">
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="E6" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2">
         <f>E6*60</f>
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="G6" s="2">
         <v>12</v>
@@ -504,19 +504,19 @@
       </c>
       <c r="J6" s="2">
         <f>I6/F6</f>
-        <v>720</v>
+        <v>144</v>
       </c>
       <c r="K6" s="3">
         <f>J6*D6</f>
-        <v>72000000</v>
+        <v>21600000</v>
       </c>
       <c r="L6" s="2">
         <f>K6/1000</f>
-        <v>72000</v>
+        <v>21600</v>
       </c>
       <c r="M6" s="2">
         <f>L6/1000</f>
-        <v>72</v>
+        <v>21.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
front back switch ok
</commit_message>
<xml_diff>
--- a/bandwith_calculation_cctv_image_android.xlsx
+++ b/bandwith_calculation_cctv_image_android.xlsx
@@ -485,11 +485,11 @@
         <v>150000</v>
       </c>
       <c r="E6" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2">
         <f>E6*60</f>
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="G6" s="2">
         <v>12</v>
@@ -504,19 +504,19 @@
       </c>
       <c r="J6" s="2">
         <f>I6/F6</f>
-        <v>144</v>
+        <v>360</v>
       </c>
       <c r="K6" s="3">
         <f>J6*D6</f>
-        <v>21600000</v>
+        <v>54000000</v>
       </c>
       <c r="L6" s="2">
         <f>K6/1000</f>
-        <v>21600</v>
+        <v>54000</v>
       </c>
       <c r="M6" s="2">
         <f>L6/1000</f>
-        <v>21.6</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>